<commit_message>
Use min_row instead of of row_offset (which is removed in newer versions of openpyxl).
</commit_message>
<xml_diff>
--- a/data/sample-hw03p3.xlsx
+++ b/data/sample-hw03p3.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65D5D98-E0E9-4B62-B0D2-416DA9BB8387}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B8646B2-00A2-4C45-985F-B9DF8B0D1A24}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -590,7 +590,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0.15</v>
+        <v>0.08</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -624,7 +624,7 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>0.15</v>
+        <v>0.08</v>
       </c>
       <c r="E4">
         <v>0</v>

</xml_diff>